<commit_message>
Added Flagellation Added Masochism AutoIgnored Default Common cards
</commit_message>
<xml_diff>
--- a/DesignDoc.xlsx
+++ b/DesignDoc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zacc\Documents\StS Modding\StS-DefaultModBase-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85F272E0-E206-43AC-A355-57AD637FA17E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD12CF03-6BF0-4B87-9CE6-9950F2E6D65D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{810DA3B1-C32A-4683-9C56-556E1105B840}"/>
+    <workbookView xWindow="6945" yWindow="1995" windowWidth="17220" windowHeight="12750" xr2:uid="{810DA3B1-C32A-4683-9C56-556E1105B840}"/>
   </bookViews>
   <sheets>
     <sheet name="Card Slots" sheetId="4" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="156">
   <si>
     <t>Character Name</t>
   </si>
@@ -254,9 +254,6 @@
     <t>Seeing Red</t>
   </si>
   <si>
-    <t>BloodlettingBrutality</t>
-  </si>
-  <si>
     <t>Reckless Charge</t>
   </si>
   <si>
@@ -414,6 +411,99 @@
   </si>
   <si>
     <t>Renounce deck</t>
+  </si>
+  <si>
+    <t>Common</t>
+  </si>
+  <si>
+    <t>Uncommon</t>
+  </si>
+  <si>
+    <t>Large Expensive Damage</t>
+  </si>
+  <si>
+    <t>Rough Description</t>
+  </si>
+  <si>
+    <t>LD Power</t>
+  </si>
+  <si>
+    <t>Smoke Screen</t>
+  </si>
+  <si>
+    <t>Soul Strike</t>
+  </si>
+  <si>
+    <t>Bloodletting</t>
+  </si>
+  <si>
+    <t>Brutality</t>
+  </si>
+  <si>
+    <t>Starter</t>
+  </si>
+  <si>
+    <t>Scales itself in combat</t>
+  </si>
+  <si>
+    <t>Next time you play a pick a path card, get both</t>
+  </si>
+  <si>
+    <t>Scales with Strength</t>
+  </si>
+  <si>
+    <t>Card Selection</t>
+  </si>
+  <si>
+    <t>Cheap attack w 'downside'</t>
+  </si>
+  <si>
+    <t>Card draw w downside</t>
+  </si>
+  <si>
+    <t>Mana</t>
+  </si>
+  <si>
+    <t>Exhaust Armor</t>
+  </si>
+  <si>
+    <t>Armor</t>
+  </si>
+  <si>
+    <t>Damage</t>
+  </si>
+  <si>
+    <t>Attack w 'downside'</t>
+  </si>
+  <si>
+    <t>Damage (draw)</t>
+  </si>
+  <si>
+    <t>Aoe &amp; AOE Debuff</t>
+  </si>
+  <si>
+    <t>Multi attack</t>
+  </si>
+  <si>
+    <t>Temp Strength</t>
+  </si>
+  <si>
+    <t>Conditional Damage</t>
+  </si>
+  <si>
+    <t>Block with ""</t>
+  </si>
+  <si>
+    <t>Block (draw)</t>
+  </si>
+  <si>
+    <t>Block and Damage</t>
+  </si>
+  <si>
+    <t>Aoe</t>
+  </si>
+  <si>
+    <t>~Vampire Bat</t>
   </si>
 </sst>
 </file>
@@ -429,15 +519,33 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE09090"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE6D870"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC1E2E9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -454,19 +562,42 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFC1E2E9"/>
+      <color rgb="FFE6D870"/>
+      <color rgb="FFD5B35D"/>
+      <color rgb="FFFBD637"/>
+      <color rgb="FFE09090"/>
+      <color rgb="FFFF7C80"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -775,400 +906,701 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCA986D6-E9D6-4B2C-895B-951A495A36D0}">
-  <dimension ref="A1:D73"/>
+  <dimension ref="A1:E74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D1" t="s">
-        <v>119</v>
+      <c r="A1" s="5"/>
+      <c r="B1" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="3" t="s">
         <v>44</v>
       </c>
       <c r="B2" t="s">
         <v>45</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="3" t="s">
         <v>44</v>
       </c>
       <c r="B3" t="s">
         <v>47</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>48</v>
       </c>
       <c r="D3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C4" t="s">
+      <c r="A4" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C5" t="s">
+      <c r="A5" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C6" t="s">
+      <c r="A6" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C7" t="s">
+      <c r="A7" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C8" t="s">
+      <c r="A8" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C9" t="s">
+      <c r="A9" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C10" t="s">
+      <c r="A10" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C11" t="s">
+      <c r="A11" t="s">
+        <v>125</v>
+      </c>
+      <c r="B11" t="s">
+        <v>152</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C12" t="s">
+      <c r="A12" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C13" t="s">
+      <c r="A13" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C14" t="s">
+      <c r="A14" t="s">
+        <v>125</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C15" t="s">
+      <c r="A15" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C16" t="s">
+      <c r="A16" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C17" t="s">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C18" t="s">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C19" t="s">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C20" t="s">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="21" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C21" t="s">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21" t="s">
+        <v>127</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="22" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C22" t="s">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>125</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="23" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C23" t="s">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="24" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C24" t="s">
+      <c r="D23" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="B24" t="s">
+        <v>143</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="25" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C25" t="s">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="B25" t="s">
+        <v>142</v>
+      </c>
+      <c r="C25" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="26" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C26" t="s">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="B26" t="s">
+        <v>141</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="27" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C27" t="s">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B28" t="s">
+        <v>140</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>125</v>
+      </c>
+      <c r="B29" t="s">
+        <v>139</v>
+      </c>
+      <c r="C29" s="2" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="28" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C28" t="s">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>125</v>
+      </c>
+      <c r="B30" t="s">
+        <v>138</v>
+      </c>
+      <c r="C30" s="2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="29" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C29" t="s">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>125</v>
+      </c>
+      <c r="C31" s="2" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="30" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C30" t="s">
+      <c r="E31" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>125</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="31" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C31" t="s">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C33" s="2" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="32" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C32" t="s">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>125</v>
+      </c>
+      <c r="C34" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C33" t="s">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C35" s="2" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C34" t="s">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C36" s="2" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="35" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C35" t="s">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>125</v>
+      </c>
+      <c r="B37" t="s">
+        <v>144</v>
+      </c>
+      <c r="C37" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="36" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C36" t="s">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>125</v>
+      </c>
+      <c r="B38" t="s">
+        <v>145</v>
+      </c>
+      <c r="C38" s="2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="37" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C37" t="s">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>134</v>
+      </c>
+      <c r="C39" s="2" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="38" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C38" t="s">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>125</v>
+      </c>
+      <c r="B40" t="s">
+        <v>154</v>
+      </c>
+      <c r="C40" s="2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="39" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C39" t="s">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C41" s="2" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="40" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C40" t="s">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C42" s="2" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="41" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C41" t="s">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>125</v>
+      </c>
+      <c r="B43" t="s">
+        <v>137</v>
+      </c>
+      <c r="C43" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="42" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C42" t="s">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C44" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="43" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C43" t="s">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>125</v>
+      </c>
+      <c r="B45" t="s">
+        <v>153</v>
+      </c>
+      <c r="C45" s="2" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="44" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C44" t="s">
+      <c r="D45" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C46" s="2" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="45" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C45" t="s">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C47" s="2" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="46" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C46" t="s">
+      <c r="D47" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="B48" t="s">
+        <v>148</v>
+      </c>
+      <c r="C48" s="2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="47" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C47" t="s">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="B49" t="s">
+        <v>135</v>
+      </c>
+      <c r="C49" s="2" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="48" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C48" t="s">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>125</v>
+      </c>
+      <c r="B50" t="s">
+        <v>147</v>
+      </c>
+      <c r="C50" s="2" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="49" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C49" t="s">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>125</v>
+      </c>
+      <c r="B51" t="s">
+        <v>151</v>
+      </c>
+      <c r="C51" s="2" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="50" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C50" t="s">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C52" s="2" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="51" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C51" t="s">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>125</v>
+      </c>
+      <c r="C53" s="2" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="52" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C52" t="s">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C54" s="2" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="53" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C53" t="s">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>125</v>
+      </c>
+      <c r="C55" s="2" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="54" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C54" t="s">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>125</v>
+      </c>
+      <c r="B56" t="s">
+        <v>146</v>
+      </c>
+      <c r="C56" s="2" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="55" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C55" t="s">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C57" s="2" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="56" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C56" t="s">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>125</v>
+      </c>
+      <c r="C58" s="2" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="57" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C57" t="s">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C59" s="2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="58" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C58" t="s">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C60" s="2" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="59" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C59" t="s">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C61" s="2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="60" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C60" t="s">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C62" s="2" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="61" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C61" t="s">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C63" s="2" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="62" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C62" t="s">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C64" s="2" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="63" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C63" t="s">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C65" s="2" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="64" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C64" t="s">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C66" s="2" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="65" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C65" t="s">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C67" s="2" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="66" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C66" t="s">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>125</v>
+      </c>
+      <c r="B68" t="s">
+        <v>149</v>
+      </c>
+      <c r="C68" s="2" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="67" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C67" t="s">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C69" s="2" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="68" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C68" t="s">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>125</v>
+      </c>
+      <c r="B70" t="s">
+        <v>150</v>
+      </c>
+      <c r="C70" s="2" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="69" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C69" t="s">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C71" s="2" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="70" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C70" t="s">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C72" s="2" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="71" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C71" t="s">
+      <c r="D72" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C73" s="2" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="72" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C72" t="s">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C74" s="2" t="s">
         <v>117</v>
-      </c>
-    </row>
-    <row r="73" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C73" t="s">
-        <v>118</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1220,27 +1652,27 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Dark Ritual Enabled StrDex power Added Escalating Strike with Strike Damage power Added Punish Weakness Fixed Burning Blood never triggering Added Soul Guard w EOT soul heal power Fixed Pain Gain splitting into the wrong cards Fixed Smoke Patch with thorns/hp loss Added Convalesce Made some numbers tweaks Added test cycle card Added punish weakness
</commit_message>
<xml_diff>
--- a/DesignDoc.xlsx
+++ b/DesignDoc.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zacc\Documents\StS Modding\StS-DefaultModBase-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6EC0DCC-523C-4F54-A509-F309A031F4CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2F89F96-1FBA-483B-B88B-20CE68E5E2BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{810DA3B1-C32A-4683-9C56-556E1105B840}"/>
+    <workbookView xWindow="10770" yWindow="1860" windowWidth="14235" windowHeight="12750" firstSheet="1" activeTab="1" xr2:uid="{810DA3B1-C32A-4683-9C56-556E1105B840}"/>
   </bookViews>
   <sheets>
     <sheet name="(Ironclad) Card Slots" sheetId="4" r:id="rId1"/>
-    <sheet name="Mechanics" sheetId="1" r:id="rId2"/>
-    <sheet name="Archetypes" sheetId="5" r:id="rId3"/>
-    <sheet name="Names and Flavour" sheetId="3" r:id="rId4"/>
+    <sheet name="Cards" sheetId="6" r:id="rId2"/>
+    <sheet name="Mechanics" sheetId="1" r:id="rId3"/>
+    <sheet name="Archetypes" sheetId="5" r:id="rId4"/>
+    <sheet name="Names and Flavour" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="265">
   <si>
     <t>Character Name</t>
   </si>
@@ -684,13 +685,160 @@
   </si>
   <si>
     <t>If the card with cycling is in your hand at the end of your turn, draw an extra card next turn</t>
+  </si>
+  <si>
+    <t>Draw Block</t>
+  </si>
+  <si>
+    <t>Draw Damage</t>
+  </si>
+  <si>
+    <t>Burnout</t>
+  </si>
+  <si>
+    <t>Stone to Flesh</t>
+  </si>
+  <si>
+    <t>Light Attack</t>
+  </si>
+  <si>
+    <t>Dark Block</t>
+  </si>
+  <si>
+    <t>Text</t>
+  </si>
+  <si>
+    <t>10 dmg 2 cards</t>
+  </si>
+  <si>
+    <t>10 block 2 cards</t>
+  </si>
+  <si>
+    <t>Deal Light damage, reduce light by one, repeat. Exhaust.</t>
+  </si>
+  <si>
+    <t>Block becomes soul health</t>
+  </si>
+  <si>
+    <t>Vampire Bat</t>
+  </si>
+  <si>
+    <t>6 + Light Attack</t>
+  </si>
+  <si>
+    <t>5 + Dark Block</t>
+  </si>
+  <si>
+    <t>6 dmg, soul heal 2</t>
+  </si>
+  <si>
+    <t>3 dmg, soul heal 1</t>
+  </si>
+  <si>
+    <t>Fog</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Gain 4X Smoke</t>
+  </si>
+  <si>
+    <t>Gain 9 Smoke</t>
+  </si>
+  <si>
+    <t>Penance</t>
+  </si>
+  <si>
+    <t>Gain 4 Thorns</t>
+  </si>
+  <si>
+    <t>Reprisal</t>
+  </si>
+  <si>
+    <t>Deal damage equal to the damage the opponent would deal</t>
+  </si>
+  <si>
+    <t>Thrashing</t>
+  </si>
+  <si>
+    <t>Gain 2 Thorns each turn</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Love playing with this card</t>
+  </si>
+  <si>
+    <t>Solid simple card, I like the numbers</t>
+  </si>
+  <si>
+    <t>Good card, I think this is in the right place</t>
+  </si>
+  <si>
+    <t>Will need to fudge the numbers as I work out the light/dark mechanic and the base relic</t>
+  </si>
+  <si>
+    <t>Not sure if I love the smoke mechanic but I really like the X smoke spell</t>
+  </si>
+  <si>
+    <t>Weird to arrange this to not be too strong or too weak, smoke is a situational mechanic</t>
+  </si>
+  <si>
+    <t>Cycle</t>
+  </si>
+  <si>
+    <t>Supplant</t>
+  </si>
+  <si>
+    <t>Oust</t>
+  </si>
+  <si>
+    <t>Ends in hand</t>
+  </si>
+  <si>
+    <t>Does X effect if the card ends the turn in your hand</t>
+  </si>
+  <si>
+    <t>Idle</t>
+  </si>
+  <si>
+    <t>Neglect</t>
+  </si>
+  <si>
+    <t>Left Behind</t>
+  </si>
+  <si>
+    <t>???</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When you defeat an Elite or Boss, permanently gain one dark </t>
+  </si>
+  <si>
+    <t>Escalating Strike</t>
+  </si>
+  <si>
+    <t>Soul Guard</t>
+  </si>
+  <si>
+    <t>Convalesce</t>
+  </si>
+  <si>
+    <t>Burning Blood</t>
+  </si>
+  <si>
+    <t>StrDex Power</t>
+  </si>
+  <si>
+    <t>Purge the Sinful</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -763,6 +911,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFCD8989"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -936,7 +1091,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -956,6 +1111,9 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -965,6 +1123,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1023,6 +1182,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFCD8989"/>
       <color rgb="FFD0B4D1"/>
       <color rgb="FFD7CFD7"/>
       <color rgb="FFDDDDDD"/>
@@ -1032,7 +1192,6 @@
       <color rgb="FF986FCF"/>
       <color rgb="FFFBD637"/>
       <color rgb="FFFFB41D"/>
-      <color rgb="FFFFCC66"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1396,14 +1555,14 @@
   <sheetData>
     <row r="1" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1"/>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="20" t="s">
         <v>145</v>
       </c>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="22"/>
       <c r="H1"/>
       <c r="I1"/>
       <c r="J1"/>
@@ -3110,11 +3269,268 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D547447-4926-4481-8423-F6A5FE392DD4}">
+  <dimension ref="A1:D26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17" customWidth="1"/>
+    <col min="2" max="2" width="33.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>242</v>
+      </c>
+      <c r="C1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D1" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="23" t="s">
+        <v>217</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="23" t="s">
+        <v>216</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>218</v>
+      </c>
+      <c r="B4" t="s">
+        <v>246</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>219</v>
+      </c>
+      <c r="B5" t="s">
+        <v>245</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>127</v>
+      </c>
+      <c r="B6" t="s">
+        <v>244</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>220</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>221</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>227</v>
+      </c>
+      <c r="B9" t="s">
+        <v>243</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>232</v>
+      </c>
+      <c r="B10" t="s">
+        <v>247</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>233</v>
+      </c>
+      <c r="D10" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>126</v>
+      </c>
+      <c r="B11" t="s">
+        <v>248</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>236</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>238</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>240</v>
+      </c>
+      <c r="C14">
+        <v>3</v>
+      </c>
+      <c r="D14" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>257</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="D16" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="23" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="23" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="23" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="23" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="23" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>264</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA4234A8-B700-4C1E-8E98-8A7AFDFE53C4}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3192,12 +3608,20 @@
         <v>215</v>
       </c>
     </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>252</v>
+      </c>
+      <c r="C12" t="s">
+        <v>253</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56A04FBC-B621-4E16-AFA8-4D9846FF85EC}">
   <dimension ref="A1:A5"/>
   <sheetViews>
@@ -3240,12 +3664,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95061868-5DC1-450C-B0FA-CC89F041A52E}">
-  <dimension ref="A1:P7"/>
+  <dimension ref="A1:P9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3425,6 +3849,31 @@
         <v>40</v>
       </c>
     </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="B8" t="s">
+        <v>250</v>
+      </c>
+      <c r="C8" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>252</v>
+      </c>
+      <c r="B9" t="s">
+        <v>254</v>
+      </c>
+      <c r="C9" t="s">
+        <v>255</v>
+      </c>
+      <c r="D9" t="s">
+        <v>256</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>